<commit_message>
- minor corrections in BOM and LDO schematic
</commit_message>
<xml_diff>
--- a/MJ808 clone - all driver- POC - BOM.xlsx
+++ b/MJ808 clone - all driver- POC - BOM.xlsx
@@ -1271,7 +1271,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:XFD35"/>
+      <selection activeCell="H35" sqref="H35:I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2054,10 +2054,10 @@
       <c r="F35" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="G35" s="4" t="s">
+      <c r="H35" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="H35" s="6" t="s">
+      <c r="I35" s="6" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2094,7 +2094,7 @@
     <hyperlink ref="I32" r:id="rId29"/>
     <hyperlink ref="I19" r:id="rId30"/>
     <hyperlink ref="I20" r:id="rId31"/>
-    <hyperlink ref="H35" r:id="rId32"/>
+    <hyperlink ref="I35" r:id="rId32"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
- corrected minor mistake in BOM
</commit_message>
<xml_diff>
--- a/MJ808 clone - all driver- POC - BOM.xlsx
+++ b/MJ808 clone - all driver- POC - BOM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="132">
   <si>
     <t>Part</t>
   </si>
@@ -253,12 +253,6 @@
     <t>https://hr.mouser.com/ProductDetail/KEMET/C0402C105K4PACTU/?qs=sGAEpiMZZMs0AnBnWHyRQJGXZSL2p4w0IWztnEtEgXr2QXa2ozRqtA%3d%3d</t>
   </si>
   <si>
-    <t xml:space="preserve">604-AM2520SURC03 </t>
-  </si>
-  <si>
-    <t>https://hr.mouser.com/ProductDetail/604-AM2520SURC03</t>
-  </si>
-  <si>
     <t>581-PRQV8.00CR1510Y</t>
   </si>
   <si>
@@ -404,6 +398,18 @@
   </si>
   <si>
     <t>https://hr.mouser.com/ProductDetail/612-TL3305CF160QG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">556-ATTINY4313-MMHR </t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/556-ATTINY4313-MMHR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">771-PMEG2010ER115 </t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/Nexperia/PMEG2010ER115?qs=%2fha2pyFaduiWO3i5eIlfQWEwBcBz4vns6cjIVfREp8qIF%2fTo2tcnsg%3d%3d</t>
   </si>
 </sst>
 </file>
@@ -1299,8 +1305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1332,7 +1338,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>74</v>
@@ -1340,418 +1346,415 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="B2" s="8">
-        <v>5034800600</v>
-      </c>
-      <c r="C2" s="8">
-        <v>5034800600</v>
+        <v>5</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>6</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>27</v>
+        <v>7</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>124</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>125</v>
+        <v>77</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>35</v>
+        <v>7</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>38</v>
+        <v>104</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>38</v>
+        <v>105</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>39</v>
+        <v>106</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>85</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>86</v>
+        <v>116</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>76</v>
+        <v>115</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>27</v>
+        <v>15</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>81</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>82</v>
+        <v>118</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>17</v>
+        <v>75</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>22</v>
+        <v>115</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>24</v>
+        <v>15</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>79</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>80</v>
+        <v>118</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>114</v>
+        <v>17</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>114</v>
+        <v>18</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>115</v>
+        <v>19</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>126</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>127</v>
+        <v>130</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>110</v>
+        <v>21</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>111</v>
+        <v>22</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>112</v>
+        <v>23</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="E9" s="8">
-        <v>311020004</v>
+        <v>24</v>
       </c>
       <c r="F9" t="s">
         <v>128</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="1" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="B10" s="8">
-        <v>120</v>
+        <v>25</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>76</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>72</v>
+        <v>26</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="F10" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="B11" s="8">
-        <v>330</v>
+        <v>28</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="F11" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="B12" s="8">
-        <v>330</v>
+        <v>32</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="F12" t="s">
-        <v>93</v>
+        <v>120</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>94</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="B13" s="8">
-        <v>330</v>
+        <v>36</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="F13" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="F14" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>56</v>
+        <v>107</v>
+      </c>
+      <c r="B15" s="8">
+        <v>5034800600</v>
+      </c>
+      <c r="C15" s="8">
+        <v>5034800600</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="F15" t="s">
-        <v>91</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>92</v>
+        <v>122</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>62</v>
+        <v>108</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>55</v>
+        <v>109</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>56</v>
+        <v>110</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>58</v>
+        <v>111</v>
+      </c>
+      <c r="E16" s="8">
+        <v>311020004</v>
       </c>
       <c r="F16" t="s">
-        <v>91</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>92</v>
+        <v>126</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="F17" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>55</v>
+        <v>112</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>56</v>
+        <v>112</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>58</v>
+        <v>113</v>
       </c>
       <c r="F18" t="s">
-        <v>91</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>92</v>
+        <v>124</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F19" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>41</v>
+        <v>57</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>58</v>
       </c>
       <c r="F20" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -1771,274 +1774,275 @@
         <v>58</v>
       </c>
       <c r="F21" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>50</v>
+        <v>68</v>
+      </c>
+      <c r="B22" s="8">
+        <v>120</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="F22" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="F23" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>75</v>
+        <v>60</v>
+      </c>
+      <c r="B24" s="8">
+        <v>330</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="F24" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>75</v>
+        <v>61</v>
+      </c>
+      <c r="B25" s="8">
+        <v>330</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="F25" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
-        <v>11</v>
+        <v>62</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>117</v>
+        <v>55</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="F26" t="s">
-        <v>120</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>121</v>
+        <v>89</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>117</v>
+        <v>63</v>
+      </c>
+      <c r="B27" s="8">
+        <v>330</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="F27" t="s">
-        <v>120</v>
-      </c>
-      <c r="G27" s="9" t="s">
-        <v>121</v>
+        <v>91</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>106</v>
+        <v>55</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>107</v>
+        <v>56</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>108</v>
+        <v>57</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="F28" t="s">
-        <v>118</v>
-      </c>
-      <c r="G28" s="9" t="s">
-        <v>119</v>
+        <v>89</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="F29" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>31</v>
+        <v>57</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>58</v>
       </c>
       <c r="F30" t="s">
-        <v>122</v>
+        <v>89</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>123</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C31" s="3">
         <v>3</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>48</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="A2:G31">
-    <sortCondition ref="F2:F31"/>
+    <sortCondition ref="A2:A31"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="G5" r:id="rId1"/>
-    <hyperlink ref="G7" r:id="rId2"/>
-    <hyperlink ref="G23" r:id="rId3"/>
-    <hyperlink ref="G24" r:id="rId4"/>
-    <hyperlink ref="G25" r:id="rId5"/>
-    <hyperlink ref="G28" r:id="rId6"/>
-    <hyperlink ref="G26" r:id="rId7"/>
-    <hyperlink ref="G27" r:id="rId8"/>
-    <hyperlink ref="G6" r:id="rId9"/>
-    <hyperlink ref="G3" r:id="rId10"/>
-    <hyperlink ref="G30" r:id="rId11"/>
-    <hyperlink ref="G4" r:id="rId12"/>
-    <hyperlink ref="G20" r:id="rId13"/>
-    <hyperlink ref="G2" r:id="rId14"/>
-    <hyperlink ref="G22" r:id="rId15"/>
-    <hyperlink ref="G14" r:id="rId16"/>
-    <hyperlink ref="G15" r:id="rId17"/>
-    <hyperlink ref="G16" r:id="rId18"/>
-    <hyperlink ref="G17" r:id="rId19"/>
-    <hyperlink ref="G18" r:id="rId20"/>
-    <hyperlink ref="G19" r:id="rId21"/>
-    <hyperlink ref="G11" r:id="rId22"/>
-    <hyperlink ref="G12" r:id="rId23"/>
-    <hyperlink ref="G13" r:id="rId24"/>
-    <hyperlink ref="G10" r:id="rId25"/>
-    <hyperlink ref="G21" r:id="rId26"/>
-    <hyperlink ref="G29" r:id="rId27"/>
-    <hyperlink ref="G31" r:id="rId28"/>
-    <hyperlink ref="G8" r:id="rId29"/>
-    <hyperlink ref="G9" r:id="rId30"/>
+    <hyperlink ref="G10" r:id="rId1"/>
+    <hyperlink ref="G2" r:id="rId2"/>
+    <hyperlink ref="G3" r:id="rId3"/>
+    <hyperlink ref="G6" r:id="rId4"/>
+    <hyperlink ref="G4" r:id="rId5"/>
+    <hyperlink ref="G5" r:id="rId6"/>
+    <hyperlink ref="G7" r:id="rId7"/>
+    <hyperlink ref="G11" r:id="rId8"/>
+    <hyperlink ref="G12" r:id="rId9"/>
+    <hyperlink ref="G13" r:id="rId10"/>
+    <hyperlink ref="G14" r:id="rId11"/>
+    <hyperlink ref="G15" r:id="rId12"/>
+    <hyperlink ref="G19" r:id="rId13"/>
+    <hyperlink ref="G20" r:id="rId14"/>
+    <hyperlink ref="G23" r:id="rId15"/>
+    <hyperlink ref="G26" r:id="rId16"/>
+    <hyperlink ref="G28" r:id="rId17"/>
+    <hyperlink ref="G29" r:id="rId18"/>
+    <hyperlink ref="G30" r:id="rId19"/>
+    <hyperlink ref="G24" r:id="rId20"/>
+    <hyperlink ref="G25" r:id="rId21"/>
+    <hyperlink ref="G27" r:id="rId22"/>
+    <hyperlink ref="G22" r:id="rId23"/>
+    <hyperlink ref="G21" r:id="rId24"/>
+    <hyperlink ref="G17" r:id="rId25"/>
+    <hyperlink ref="G31" r:id="rId26"/>
+    <hyperlink ref="G18" r:id="rId27"/>
+    <hyperlink ref="G16" r:id="rId28"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>